<commit_message>
Completed CHECK AND TRANSFER DOCUMENT TO CORRECT PATH IN CONTUR DIADOK WEBPAGE
</commit_message>
<xml_diff>
--- a/Diadok_DOCS.xlsx
+++ b/Diadok_DOCS.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="61" uniqueCount="26">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="109" uniqueCount="32">
   <si>
     <t>Саратов</t>
   </si>
@@ -79,9 +79,6 @@
     <t>17 ТЛ</t>
   </si>
   <si>
-    <t>ЦСС ОАО РЖД</t>
-  </si>
-  <si>
     <t>Ростелеком</t>
   </si>
   <si>
@@ -98,6 +95,27 @@
   </si>
   <si>
     <t>/1ЗЗ-О9</t>
+  </si>
+  <si>
+    <t>Департамент информационных технологий</t>
+  </si>
+  <si>
+    <t>Центральная станция связи ОАО «РЖД»</t>
+  </si>
+  <si>
+    <t>Служба административно-хозяйственного обеспечения</t>
+  </si>
+  <si>
+    <t>/00190</t>
+  </si>
+  <si>
+    <t>/00114</t>
+  </si>
+  <si>
+    <t>/00115</t>
+  </si>
+  <si>
+    <t>/00109</t>
   </si>
 </sst>
 </file>
@@ -419,16 +437,16 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C21"/>
+  <dimension ref="A1:C25"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D13" sqref="D13"/>
+      <selection activeCell="B15" sqref="B15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="14.140625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="23.28515625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="41.140625" customWidth="1"/>
+    <col min="2" max="2" width="53.28515625" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="30.140625" style="1" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
@@ -440,12 +458,12 @@
         <v>2</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B2" t="s">
         <v>0</v>
@@ -456,18 +474,18 @@
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B3" t="s">
         <v>0</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B4" t="s">
         <v>0</v>
@@ -478,18 +496,18 @@
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B5" t="s">
         <v>0</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B6" t="s">
         <v>0</v>
@@ -500,18 +518,18 @@
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B7" t="s">
         <v>0</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B8" t="s">
         <v>0</v>
@@ -522,17 +540,190 @@
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B9" t="s">
-        <v>2</v>
+        <v>25</v>
       </c>
       <c r="C9" s="1" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="21" spans="3:3" x14ac:dyDescent="0.25">
-      <c r="C21" s="2"/>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>26</v>
+      </c>
+      <c r="B10" t="s">
+        <v>0</v>
+      </c>
+      <c r="C10" s="1" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>26</v>
+      </c>
+      <c r="B11" t="s">
+        <v>0</v>
+      </c>
+      <c r="C11" s="1" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>26</v>
+      </c>
+      <c r="B12" t="s">
+        <v>0</v>
+      </c>
+      <c r="C12" s="1" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>26</v>
+      </c>
+      <c r="B13" t="s">
+        <v>0</v>
+      </c>
+      <c r="C13" s="1" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>26</v>
+      </c>
+      <c r="B14" t="s">
+        <v>0</v>
+      </c>
+      <c r="C14" s="1" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>26</v>
+      </c>
+      <c r="B15" t="s">
+        <v>0</v>
+      </c>
+      <c r="C15" s="1" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>26</v>
+      </c>
+      <c r="B16" t="s">
+        <v>0</v>
+      </c>
+      <c r="C16" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>26</v>
+      </c>
+      <c r="B17" t="s">
+        <v>0</v>
+      </c>
+      <c r="C17" s="1" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
+        <v>26</v>
+      </c>
+      <c r="B18" t="s">
+        <v>0</v>
+      </c>
+      <c r="C18" s="1" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
+        <v>19</v>
+      </c>
+      <c r="B19" t="s">
+        <v>0</v>
+      </c>
+      <c r="C19" s="1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
+        <v>19</v>
+      </c>
+      <c r="B20" t="s">
+        <v>0</v>
+      </c>
+      <c r="C20" s="1" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A21" t="s">
+        <v>19</v>
+      </c>
+      <c r="B21" t="s">
+        <v>0</v>
+      </c>
+      <c r="C21" s="1" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A22" t="s">
+        <v>26</v>
+      </c>
+      <c r="B22" t="s">
+        <v>25</v>
+      </c>
+      <c r="C22" s="1" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A23" t="s">
+        <v>20</v>
+      </c>
+      <c r="B23" t="s">
+        <v>25</v>
+      </c>
+      <c r="C23" s="1" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A24" t="s">
+        <v>26</v>
+      </c>
+      <c r="B24" t="s">
+        <v>27</v>
+      </c>
+      <c r="C24" s="2" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A25" t="s">
+        <v>26</v>
+      </c>
+      <c r="B25" t="s">
+        <v>27</v>
+      </c>
+      <c r="C25" s="1" t="s">
+        <v>18</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -545,14 +736,17 @@
   <dimension ref="A1:C12"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C10" sqref="A10:C10"/>
+      <selection sqref="A1:C12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="78.28515625" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>19</v>
+        <v>26</v>
       </c>
       <c r="B1" t="s">
         <v>0</v>
@@ -563,7 +757,7 @@
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>19</v>
+        <v>26</v>
       </c>
       <c r="B2" t="s">
         <v>0</v>
@@ -574,7 +768,7 @@
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>19</v>
+        <v>26</v>
       </c>
       <c r="B3" t="s">
         <v>0</v>
@@ -585,7 +779,7 @@
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>19</v>
+        <v>26</v>
       </c>
       <c r="B4" t="s">
         <v>0</v>
@@ -596,7 +790,7 @@
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>19</v>
+        <v>26</v>
       </c>
       <c r="B5" t="s">
         <v>0</v>
@@ -607,7 +801,7 @@
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B6" t="s">
         <v>0</v>
@@ -618,7 +812,7 @@
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B7" t="s">
         <v>0</v>
@@ -629,7 +823,7 @@
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B8" t="s">
         <v>0</v>
@@ -640,7 +834,7 @@
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>19</v>
+        <v>26</v>
       </c>
       <c r="B9" t="s">
         <v>2</v>
@@ -651,7 +845,7 @@
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B10" t="s">
         <v>2</v>
@@ -662,7 +856,7 @@
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>19</v>
+        <v>26</v>
       </c>
       <c r="B11" t="s">
         <v>3</v>
@@ -673,7 +867,7 @@
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>19</v>
+        <v>26</v>
       </c>
       <c r="B12" t="s">
         <v>3</v>

</xml_diff>